<commit_message>
membuat model ke 2
</commit_message>
<xml_diff>
--- a/public/DaftarKegiatanData/uji coba.xlsx
+++ b/public/DaftarKegiatanData/uji coba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilham Dio Putra\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB843B9-A1C0-4562-82ED-3D96474CC3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2D9D03-95E0-43F5-B375-FE746ADDF57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,19 +42,19 @@
     <t>12 / 12 Bulan Layanan</t>
   </si>
   <si>
-    <t>4471.DBA.003.051.B FDUN.BLU.006</t>
-  </si>
-  <si>
-    <t>Gaji Karyawan Non PNS</t>
-  </si>
-  <si>
     <t>4.1.1 Kerjasama dengan mitra</t>
   </si>
   <si>
-    <t>4471.DBA.001.060.GB FDUN.BLU.019</t>
-  </si>
-  <si>
-    <t>Biaya Kerjasama pengampuan dan Institusional fee FK UNDIP</t>
+    <t>Aaaaaa</t>
+  </si>
+  <si>
+    <t>bbbbbbbbb</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaaaaaa</t>
   </si>
 </sst>
 </file>
@@ -118,11 +118,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -136,6 +133,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +446,7 @@
   <dimension ref="B1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,31 +460,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4">
-        <v>150000000</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="3">
+        <v>20000</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -490,9 +493,9 @@
         <v>2</v>
       </c>
       <c r="F2">
-        <v>471000000</v>
-      </c>
-      <c r="G2" s="6" t="s">
+        <v>5000000</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>